<commit_message>
Registrar Materias funciona y mejorado el main
</commit_message>
<xml_diff>
--- a/data/Currículo ISIS.xlsx
+++ b/data/Currículo ISIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Juan PC\Documents\Programming Scripts\Java Scripts\Proyecto 1 DPOO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDA6362-A53D-4DB3-91BA-8F75333F5D83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853FF962-27FD-4E79-8C88-3E1E7088225C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B506AC9-E6CF-4073-A3EA-BFD6E37016C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="119">
   <si>
     <t>Nombre Materia</t>
   </si>
@@ -385,6 +385,12 @@
   </si>
   <si>
     <t>Electiva en Ciencias</t>
+  </si>
+  <si>
+    <t>CBXX-XXXX</t>
+  </si>
+  <si>
+    <t>Curso de Libre Elección</t>
   </si>
 </sst>
 </file>
@@ -753,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B9106A-A628-4F6D-A335-66F36ACF90F9}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +772,7 @@
     <col min="3" max="3" width="55.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1787,6 +1793,9 @@
       <c r="B40" t="s">
         <v>96</v>
       </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
       <c r="D40" t="s">
         <v>7</v>
       </c>
@@ -1807,6 +1816,9 @@
       <c r="A41" t="s">
         <v>86</v>
       </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
@@ -1851,10 +1863,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" t="s">
-        <v>96</v>
+        <v>118</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -1863,10 +1875,10 @@
         <v>3</v>
       </c>
       <c r="F43">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="H43" t="s">
         <v>110</v>
@@ -1874,10 +1886,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -1886,13 +1898,13 @@
         <v>7</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="H44" t="s">
         <v>110</v>
@@ -1902,6 +1914,9 @@
       <c r="A45" t="s">
         <v>42</v>
       </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
@@ -1923,22 +1938,22 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B46" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H46" t="s">
         <v>110</v>
@@ -1946,22 +1961,25 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>117</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F47">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="H47" t="s">
         <v>110</v>
@@ -1969,25 +1987,25 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F48">
         <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H48" t="s">
         <v>110</v>
@@ -1995,7 +2013,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -2004,13 +2025,13 @@
         <v>7</v>
       </c>
       <c r="E49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G49" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="H49" t="s">
         <v>110</v>
@@ -2018,24 +2039,79 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>113</v>
+      </c>
+      <c r="H50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>42</v>
       </c>
-      <c r="C50" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50">
+      <c r="B51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51">
         <v>2</v>
       </c>
-      <c r="F50">
+      <c r="F51">
         <v>0</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G51" t="s">
         <v>42</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>42</v>
+      </c>
+      <c r="H52" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LENG arreglado, ahora se revisa si la materia fue o no vista
</commit_message>
<xml_diff>
--- a/data/Currículo ISIS.xlsx
+++ b/data/Currículo ISIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Juan PC\Documents\Programming Scripts\Java Scripts\Proyecto 1 DPOO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853FF962-27FD-4E79-8C88-3E1E7088225C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4A5151-7A8F-4A9C-8921-8F4C309ADC23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B506AC9-E6CF-4073-A3EA-BFD6E37016C9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="118">
   <si>
     <t>Nombre Materia</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>Electiva CBU</t>
-  </si>
-  <si>
-    <t>LENG-1512|LENG1622</t>
   </si>
   <si>
     <t>CBCO-XXXX</t>
@@ -761,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B9106A-A628-4F6D-A335-66F36ACF90F9}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,13 +789,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -821,10 +818,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -847,10 +844,10 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -873,10 +870,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -899,10 +896,10 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,10 +922,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -951,10 +948,10 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -977,10 +974,10 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1003,10 +1000,10 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1029,10 +1026,10 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1055,10 +1052,10 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1081,10 +1078,10 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1107,10 +1104,10 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1118,7 +1115,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1136,7 +1133,7 @@
         <v>42</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1159,10 +1156,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1185,10 +1182,10 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1211,10 +1208,10 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,7 +1225,7 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1237,18 +1234,18 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -1263,18 +1260,18 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1289,22 +1286,22 @@
         <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
         <v>55</v>
       </c>
-      <c r="C21" t="s">
-        <v>56</v>
-      </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
@@ -1315,19 +1312,19 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
@@ -1341,21 +1338,21 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -1367,21 +1364,21 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -1393,21 +1390,21 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
         <v>68</v>
       </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -1419,21 +1416,21 @@
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -1445,18 +1442,18 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
         <v>36</v>
@@ -1471,21 +1468,21 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>61</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -1497,21 +1494,21 @@
         <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -1523,21 +1520,21 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>66</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -1549,21 +1546,21 @@
         <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
         <v>72</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -1575,21 +1572,21 @@
         <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
         <v>75</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>76</v>
-      </c>
-      <c r="C32" t="s">
-        <v>77</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -1601,21 +1598,21 @@
         <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -1627,18 +1624,18 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -1650,22 +1647,22 @@
         <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
         <v>82</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>83</v>
       </c>
-      <c r="C35" t="s">
-        <v>84</v>
-      </c>
       <c r="D35" t="s">
         <v>7</v>
       </c>
@@ -1676,22 +1673,22 @@
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
         <v>87</v>
       </c>
-      <c r="C36" t="s">
-        <v>88</v>
-      </c>
       <c r="D36" t="s">
         <v>7</v>
       </c>
@@ -1702,22 +1699,22 @@
         <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
         <v>89</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>90</v>
       </c>
-      <c r="C37" t="s">
-        <v>91</v>
-      </c>
       <c r="D37" t="s">
         <v>7</v>
       </c>
@@ -1728,22 +1725,22 @@
         <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
         <v>92</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>93</v>
       </c>
-      <c r="C38" t="s">
-        <v>94</v>
-      </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
@@ -1754,10 +1751,10 @@
         <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1765,7 +1762,7 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1783,15 +1780,15 @@
         <v>42</v>
       </c>
       <c r="H39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1806,15 +1803,15 @@
         <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -1829,22 +1826,22 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
         <v>98</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>99</v>
       </c>
-      <c r="C42" t="s">
-        <v>100</v>
-      </c>
       <c r="D42" t="s">
         <v>7</v>
       </c>
@@ -1855,15 +1852,15 @@
         <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1878,36 +1875,36 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
         <v>96</v>
       </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44">
-        <v>3</v>
-      </c>
-      <c r="F44">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>97</v>
-      </c>
       <c r="H44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1915,7 +1912,7 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
@@ -1933,12 +1930,12 @@
         <v>42</v>
       </c>
       <c r="H45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -1953,10 +1950,10 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1964,7 +1961,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
@@ -1982,19 +1979,19 @@
         <v>42</v>
       </c>
       <c r="H47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" t="s">
         <v>102</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>103</v>
       </c>
-      <c r="C48" t="s">
-        <v>104</v>
-      </c>
       <c r="D48" t="s">
         <v>7</v>
       </c>
@@ -2005,44 +2002,44 @@
         <v>3</v>
       </c>
       <c r="G48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
         <v>96</v>
       </c>
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49">
-        <v>3</v>
-      </c>
-      <c r="F49">
-        <v>3</v>
-      </c>
-      <c r="G49" t="s">
-        <v>97</v>
-      </c>
       <c r="H49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
         <v>105</v>
-      </c>
-      <c r="B50" t="s">
-        <v>106</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -2057,10 +2054,10 @@
         <v>3</v>
       </c>
       <c r="G50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2068,7 +2065,7 @@
         <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -2086,7 +2083,7 @@
         <v>42</v>
       </c>
       <c r="H51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2094,7 +2091,7 @@
         <v>42</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -2112,7 +2109,7 @@
         <v>42</v>
       </c>
       <c r="H52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>